<commit_message>
Implemented reversing the ll recursively
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1659,11 +1659,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A364" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C184" activeCellId="0" sqref="C184"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A370" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B407" activeCellId="0" sqref="B407"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3100,7 +3100,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>